<commit_message>
EPBDS-9677 Support dependency on rules from tests in OpenL Maven Plugin
--HG--
branch : 5.23.x
</commit_message>
<xml_diff>
--- a/Util/openl-maven-plugin/it/openl-multiple-deployment/openl-parent-project/src/main/openl/Project1-Main.xlsx
+++ b/Util/openl-maven-plugin/it/openl-multiple-deployment/openl-parent-project/src/main/openl/Project1-Main.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5637A6-15DC-4618-B273-ABFF49C8B12A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14EA513-0C69-42B4-BECE-303166D32C0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,22 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Steps</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Step1</t>
+  </si>
+  <si>
+    <t>Step2</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult spr(String name, Integer age)</t>
+  </si>
   <si>
     <t>Environment</t>
   </si>
@@ -31,19 +46,10 @@
     <t>Project2-*</t>
   </si>
   <si>
-    <t>Test sayHello</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>_res_</t>
-  </si>
-  <si>
-    <t>Ivan</t>
-  </si>
-  <si>
-    <t>Hello, Ivan</t>
+    <t>= "I am " + age + " age old."</t>
+  </si>
+  <si>
+    <t>= sayHello(name)</t>
   </si>
 </sst>
 </file>
@@ -81,12 +87,10 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -364,7 +368,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:D14"/>
+  <dimension ref="C4:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
@@ -376,55 +380,49 @@
     <col min="4" max="4" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C13:D13"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>